<commit_message>
Implementacao da grade horaria
</commit_message>
<xml_diff>
--- a/teste frequência/labteste/Base-folhaPonto-2025-10.xlsx
+++ b/teste frequência/labteste/Base-folhaPonto-2025-10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\General_Folders\Acadêmico_2025_2\Fatec-2025-2\PontoFatec-Formulario\teste frequência\labteste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F32496B-6E58-4FED-BCE2-CFBF8D215159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB6EC86-7694-405E-BE97-9B9B5EB70DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parametros" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="106">
   <si>
     <t>AnoBase</t>
   </si>
@@ -351,16 +351,10 @@
     <t>Aulas</t>
   </si>
   <si>
-    <t>--</t>
-  </si>
-  <si>
     <t>Prof1-1234567</t>
   </si>
   <si>
     <t>X</t>
-  </si>
-  <si>
-    <t>---</t>
   </si>
   <si>
     <t>x</t>
@@ -976,14 +970,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -992,6 +980,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1036,14 +1033,11 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="4">
     <dxf>
       <font>
         <b/>
@@ -1089,30 +1083,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2069,8 +2039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A5:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3006,8 +2976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7E9530-1B40-4B70-870D-BAB8F8FBAD7E}">
   <dimension ref="A3:WXU24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="Q24" sqref="B19:Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3042,7 +3012,7 @@
         <v>74</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:17 15483:16193" x14ac:dyDescent="0.25">
@@ -3144,12 +3114,8 @@
       <c r="I13" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="J13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>78</v>
-      </c>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
       <c r="L13" s="8"/>
       <c r="M13" s="2" t="s">
         <v>44</v>
@@ -3873,48 +3839,48 @@
     </row>
     <row r="15" spans="1:17 15483:16193" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:17 15483:16193" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="62" t="s">
+      <c r="B16" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="63"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63"/>
-      <c r="G16" s="63"/>
-      <c r="H16" s="63"/>
-      <c r="I16" s="63"/>
-      <c r="J16" s="63"/>
-      <c r="K16" s="63"/>
-      <c r="L16" s="63"/>
-      <c r="M16" s="63"/>
-      <c r="N16" s="63"/>
-      <c r="O16" s="63"/>
-      <c r="P16" s="63"/>
-      <c r="Q16" s="64"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="61"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="61"/>
+      <c r="L16" s="61"/>
+      <c r="M16" s="61"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="61"/>
+      <c r="P16" s="61"/>
+      <c r="Q16" s="62"/>
     </row>
     <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="60"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="65" t="s">
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="I17" s="66"/>
-      <c r="J17" s="66"/>
-      <c r="K17" s="66"/>
-      <c r="L17" s="66"/>
-      <c r="M17" s="67"/>
-      <c r="N17" s="68" t="s">
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="67"/>
+      <c r="M17" s="68"/>
+      <c r="N17" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="O17" s="69"/>
-      <c r="P17" s="69"/>
-      <c r="Q17" s="70"/>
+      <c r="O17" s="70"/>
+      <c r="P17" s="70"/>
+      <c r="Q17" s="71"/>
     </row>
     <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="39" t="s">
@@ -3977,49 +3943,49 @@
         <v>105</v>
       </c>
       <c r="C19" s="42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D19" s="42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E19" s="42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F19" s="42" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G19" s="46" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H19" s="38" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I19" s="38" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="J19" s="42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K19" s="42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L19" s="42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M19" s="46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N19" s="52" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="O19" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="P19" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="Q19" s="46" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4027,52 +3993,52 @@
         <v>28</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C20" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D20" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E20" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F20" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G20" s="47" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H20" s="37" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I20" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="J20" s="43" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K20" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="L20" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="M20" s="47" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="N20" s="53" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="O20" s="43" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="P20" s="43" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="Q20" s="47" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4080,52 +4046,52 @@
         <v>29</v>
       </c>
       <c r="B21" s="38" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C21" s="42" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D21" s="42" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E21" s="42" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F21" s="42" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G21" s="46" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H21" s="38" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I21" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="J21" s="42" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K21" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="L21" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="M21" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="N21" s="79" t="s">
-        <v>103</v>
+        <v>105</v>
+      </c>
+      <c r="N21" s="59" t="s">
+        <v>105</v>
       </c>
       <c r="O21" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="P21" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="Q21" s="46" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4133,52 +4099,52 @@
         <v>30</v>
       </c>
       <c r="B22" s="37" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C22" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D22" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E22" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F22" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G22" s="47" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H22" s="37" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I22" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="J22" s="43" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K22" s="43" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L22" s="43" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M22" s="47" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N22" s="53" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="O22" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="P22" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="Q22" s="47" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4186,52 +4152,52 @@
         <v>31</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C23" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D23" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E23" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F23" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G23" s="46" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H23" s="56" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I23" s="57" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="J23" s="57" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K23" s="57" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="L23" s="57" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="M23" s="58" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="N23" s="52" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="O23" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="P23" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="Q23" s="46" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4239,52 +4205,52 @@
         <v>40</v>
       </c>
       <c r="B24" s="48" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C24" s="49" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D24" s="49" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E24" s="49" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F24" s="49" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G24" s="50" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H24" s="54" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I24" s="55" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="J24" s="55" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K24" s="55" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="L24" s="55" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="M24" s="55" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="N24" s="49" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="O24" s="49" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="P24" s="49" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="Q24" s="50" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -4313,8 +4279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6249555E-CACB-4B51-8F35-5416EB9605CE}">
   <dimension ref="A3:WXU24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5180,48 +5146,48 @@
     </row>
     <row r="15" spans="1:17 15483:16193" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:17 15483:16193" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="62" t="s">
+      <c r="B16" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="63"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63"/>
-      <c r="G16" s="63"/>
-      <c r="H16" s="63"/>
-      <c r="I16" s="63"/>
-      <c r="J16" s="63"/>
-      <c r="K16" s="63"/>
-      <c r="L16" s="63"/>
-      <c r="M16" s="63"/>
-      <c r="N16" s="63"/>
-      <c r="O16" s="63"/>
-      <c r="P16" s="63"/>
-      <c r="Q16" s="64"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="61"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="61"/>
+      <c r="L16" s="61"/>
+      <c r="M16" s="61"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="61"/>
+      <c r="P16" s="61"/>
+      <c r="Q16" s="62"/>
     </row>
     <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="60"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="65" t="s">
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="I17" s="66"/>
-      <c r="J17" s="66"/>
-      <c r="K17" s="66"/>
-      <c r="L17" s="66"/>
-      <c r="M17" s="67"/>
-      <c r="N17" s="68" t="s">
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="67"/>
+      <c r="M17" s="68"/>
+      <c r="N17" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="O17" s="69"/>
-      <c r="P17" s="69"/>
-      <c r="Q17" s="70"/>
+      <c r="O17" s="70"/>
+      <c r="P17" s="70"/>
+      <c r="Q17" s="71"/>
     </row>
     <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="39" t="s">
@@ -5281,52 +5247,52 @@
         <v>27</v>
       </c>
       <c r="B19" s="38" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C19" s="42" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D19" s="42" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E19" s="42" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F19" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G19" s="46" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H19" s="38" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I19" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="J19" s="42" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="K19" s="42" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L19" s="42" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="M19" s="46" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="N19" s="52" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="O19" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="P19" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="Q19" s="46" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5334,52 +5300,52 @@
         <v>28</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C20" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D20" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E20" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F20" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G20" s="47" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H20" s="37" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I20" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="J20" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K20" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="L20" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="M20" s="47" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="N20" s="53" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="O20" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="P20" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="Q20" s="47" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5387,52 +5353,52 @@
         <v>29</v>
       </c>
       <c r="B21" s="38" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C21" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D21" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E21" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F21" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G21" s="46" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H21" s="38" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I21" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="J21" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K21" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="L21" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="M21" s="46" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="N21" s="52" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="O21" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="P21" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="Q21" s="46" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5440,52 +5406,52 @@
         <v>30</v>
       </c>
       <c r="B22" s="37" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C22" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D22" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E22" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F22" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G22" s="47" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H22" s="37" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I22" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="J22" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K22" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="L22" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="M22" s="47" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="N22" s="53" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="O22" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="P22" s="43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="Q22" s="47" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5493,52 +5459,52 @@
         <v>31</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C23" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D23" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E23" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F23" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G23" s="46" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H23" s="56" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I23" s="57" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="J23" s="57" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K23" s="57" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="L23" s="57" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="M23" s="58" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="N23" s="52" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="O23" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="P23" s="42" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="Q23" s="46" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5546,52 +5512,52 @@
         <v>40</v>
       </c>
       <c r="B24" s="48" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C24" s="49" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D24" s="49" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E24" s="49" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F24" s="49" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G24" s="50" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H24" s="54" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I24" s="55" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="J24" s="55" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K24" s="55" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="L24" s="55" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="M24" s="55" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="N24" s="49" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="O24" s="49" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="P24" s="49" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="Q24" s="50" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -5757,107 +5723,107 @@
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N10" s="71" t="s">
+      <c r="N10" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="O10" s="72"/>
-      <c r="P10" s="72"/>
-      <c r="Q10" s="72"/>
-      <c r="R10" s="72"/>
-      <c r="S10" s="72"/>
-      <c r="T10" s="72"/>
-      <c r="U10" s="72"/>
-      <c r="V10" s="72"/>
-      <c r="W10" s="72"/>
-      <c r="X10" s="72"/>
-      <c r="Y10" s="72"/>
-      <c r="Z10" s="72"/>
-      <c r="AA10" s="72"/>
-      <c r="AB10" s="72"/>
-      <c r="AC10" s="72"/>
-      <c r="AD10" s="72"/>
-      <c r="AE10" s="72"/>
-      <c r="AF10" s="72"/>
-      <c r="AG10" s="72"/>
-      <c r="AH10" s="72"/>
-      <c r="AI10" s="72"/>
-      <c r="AJ10" s="72"/>
-      <c r="AK10" s="72"/>
-      <c r="AL10" s="72"/>
-      <c r="AM10" s="72"/>
-      <c r="AN10" s="72"/>
-      <c r="AO10" s="72"/>
-      <c r="AP10" s="72"/>
-      <c r="AQ10" s="72"/>
-      <c r="AR10" s="72"/>
-      <c r="AS10" s="72"/>
-      <c r="AT10" s="72"/>
-      <c r="AU10" s="72"/>
-      <c r="AV10" s="72"/>
-      <c r="AW10" s="73"/>
-      <c r="AX10" s="74" t="s">
+      <c r="O10" s="73"/>
+      <c r="P10" s="73"/>
+      <c r="Q10" s="73"/>
+      <c r="R10" s="73"/>
+      <c r="S10" s="73"/>
+      <c r="T10" s="73"/>
+      <c r="U10" s="73"/>
+      <c r="V10" s="73"/>
+      <c r="W10" s="73"/>
+      <c r="X10" s="73"/>
+      <c r="Y10" s="73"/>
+      <c r="Z10" s="73"/>
+      <c r="AA10" s="73"/>
+      <c r="AB10" s="73"/>
+      <c r="AC10" s="73"/>
+      <c r="AD10" s="73"/>
+      <c r="AE10" s="73"/>
+      <c r="AF10" s="73"/>
+      <c r="AG10" s="73"/>
+      <c r="AH10" s="73"/>
+      <c r="AI10" s="73"/>
+      <c r="AJ10" s="73"/>
+      <c r="AK10" s="73"/>
+      <c r="AL10" s="73"/>
+      <c r="AM10" s="73"/>
+      <c r="AN10" s="73"/>
+      <c r="AO10" s="73"/>
+      <c r="AP10" s="73"/>
+      <c r="AQ10" s="73"/>
+      <c r="AR10" s="73"/>
+      <c r="AS10" s="73"/>
+      <c r="AT10" s="73"/>
+      <c r="AU10" s="73"/>
+      <c r="AV10" s="73"/>
+      <c r="AW10" s="74"/>
+      <c r="AX10" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="AY10" s="75"/>
-      <c r="AZ10" s="75"/>
-      <c r="BA10" s="75"/>
-      <c r="BB10" s="75"/>
-      <c r="BC10" s="75"/>
-      <c r="BD10" s="75"/>
-      <c r="BE10" s="75"/>
-      <c r="BF10" s="75"/>
-      <c r="BG10" s="75"/>
-      <c r="BH10" s="75"/>
-      <c r="BI10" s="75"/>
-      <c r="BJ10" s="75"/>
-      <c r="BK10" s="75"/>
-      <c r="BL10" s="75"/>
-      <c r="BM10" s="75"/>
-      <c r="BN10" s="75"/>
-      <c r="BO10" s="75"/>
-      <c r="BP10" s="75"/>
-      <c r="BQ10" s="75"/>
-      <c r="BR10" s="75"/>
-      <c r="BS10" s="75"/>
-      <c r="BT10" s="75"/>
-      <c r="BU10" s="75"/>
-      <c r="BV10" s="75"/>
-      <c r="BW10" s="75"/>
-      <c r="BX10" s="75"/>
-      <c r="BY10" s="75"/>
-      <c r="BZ10" s="75"/>
-      <c r="CA10" s="75"/>
-      <c r="CB10" s="75"/>
-      <c r="CC10" s="75"/>
-      <c r="CD10" s="75"/>
-      <c r="CE10" s="75"/>
-      <c r="CF10" s="75"/>
-      <c r="CG10" s="76"/>
-      <c r="CH10" s="77" t="s">
+      <c r="AY10" s="76"/>
+      <c r="AZ10" s="76"/>
+      <c r="BA10" s="76"/>
+      <c r="BB10" s="76"/>
+      <c r="BC10" s="76"/>
+      <c r="BD10" s="76"/>
+      <c r="BE10" s="76"/>
+      <c r="BF10" s="76"/>
+      <c r="BG10" s="76"/>
+      <c r="BH10" s="76"/>
+      <c r="BI10" s="76"/>
+      <c r="BJ10" s="76"/>
+      <c r="BK10" s="76"/>
+      <c r="BL10" s="76"/>
+      <c r="BM10" s="76"/>
+      <c r="BN10" s="76"/>
+      <c r="BO10" s="76"/>
+      <c r="BP10" s="76"/>
+      <c r="BQ10" s="76"/>
+      <c r="BR10" s="76"/>
+      <c r="BS10" s="76"/>
+      <c r="BT10" s="76"/>
+      <c r="BU10" s="76"/>
+      <c r="BV10" s="76"/>
+      <c r="BW10" s="76"/>
+      <c r="BX10" s="76"/>
+      <c r="BY10" s="76"/>
+      <c r="BZ10" s="76"/>
+      <c r="CA10" s="76"/>
+      <c r="CB10" s="76"/>
+      <c r="CC10" s="76"/>
+      <c r="CD10" s="76"/>
+      <c r="CE10" s="76"/>
+      <c r="CF10" s="76"/>
+      <c r="CG10" s="77"/>
+      <c r="CH10" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="CI10" s="78"/>
-      <c r="CJ10" s="78"/>
-      <c r="CK10" s="78"/>
-      <c r="CL10" s="78"/>
-      <c r="CM10" s="78"/>
-      <c r="CN10" s="78"/>
-      <c r="CO10" s="78"/>
-      <c r="CP10" s="78"/>
-      <c r="CQ10" s="78"/>
-      <c r="CR10" s="78"/>
-      <c r="CS10" s="78"/>
-      <c r="CT10" s="78"/>
-      <c r="CU10" s="78"/>
-      <c r="CV10" s="78"/>
-      <c r="CW10" s="78"/>
-      <c r="CX10" s="78"/>
-      <c r="CY10" s="78"/>
-      <c r="CZ10" s="78"/>
-      <c r="DA10" s="78"/>
-      <c r="DB10" s="78"/>
-      <c r="DC10" s="78"/>
-      <c r="DD10" s="78"/>
+      <c r="CI10" s="79"/>
+      <c r="CJ10" s="79"/>
+      <c r="CK10" s="79"/>
+      <c r="CL10" s="79"/>
+      <c r="CM10" s="79"/>
+      <c r="CN10" s="79"/>
+      <c r="CO10" s="79"/>
+      <c r="CP10" s="79"/>
+      <c r="CQ10" s="79"/>
+      <c r="CR10" s="79"/>
+      <c r="CS10" s="79"/>
+      <c r="CT10" s="79"/>
+      <c r="CU10" s="79"/>
+      <c r="CV10" s="79"/>
+      <c r="CW10" s="79"/>
+      <c r="CX10" s="79"/>
+      <c r="CY10" s="79"/>
+      <c r="CZ10" s="79"/>
+      <c r="DA10" s="79"/>
+      <c r="DB10" s="79"/>
+      <c r="DC10" s="79"/>
+      <c r="DD10" s="79"/>
       <c r="DE10" s="2" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Avanço na grade de horario: de sinalização da aula no dia da semana á sinalizacao de  feriado
</commit_message>
<xml_diff>
--- a/teste frequência/labteste/Base-folhaPonto-2025-10.xlsx
+++ b/teste frequência/labteste/Base-folhaPonto-2025-10.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\General_Folders\Acadêmico_2025_2\Fatec-2025-2\PontoFatec-Formulario\teste frequência\labteste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB6EC86-7694-405E-BE97-9B9B5EB70DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E868F7FD-B864-47BD-A730-815B6A907C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parametros" sheetId="1" r:id="rId1"/>
-    <sheet name="calendario" sheetId="2" r:id="rId2"/>
-    <sheet name="Prof1-1234567" sheetId="3" r:id="rId3"/>
-    <sheet name="Prof2-1234568" sheetId="5" r:id="rId4"/>
-    <sheet name="BKP" sheetId="4" r:id="rId5"/>
+    <sheet name="feriados" sheetId="2" r:id="rId2"/>
+    <sheet name="CalendarioRemotas" sheetId="7" r:id="rId3"/>
+    <sheet name="Prof1-1234567" sheetId="3" r:id="rId4"/>
+    <sheet name="Prof2-1234568" sheetId="5" r:id="rId5"/>
+    <sheet name="BKP" sheetId="4" r:id="rId6"/>
+    <sheet name="calendario (2)" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="129">
   <si>
     <t>AnoBase</t>
   </si>
@@ -198,12 +200,6 @@
     <t>H</t>
   </si>
   <si>
-    <t>Dia</t>
-  </si>
-  <si>
-    <t>Semana</t>
-  </si>
-  <si>
     <t>Qui</t>
   </si>
   <si>
@@ -359,12 +355,87 @@
   <si>
     <t>x</t>
   </si>
+  <si>
+    <t>Dia da Semana</t>
+  </si>
+  <si>
+    <t>Dia do Mês</t>
+  </si>
+  <si>
+    <t>Tabela de feriado do Mês</t>
+  </si>
+  <si>
+    <t>Descricao do Feriado</t>
+  </si>
+  <si>
+    <t>Emenda de feriado</t>
+  </si>
+  <si>
+    <t>----</t>
+  </si>
+  <si>
+    <t>Dia do professor</t>
+  </si>
+  <si>
+    <t>Feriado ficticio</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dia da Semana </t>
+  </si>
+  <si>
+    <t>Disciplinas Híbridas do Professor</t>
+  </si>
+  <si>
+    <t>Periodo</t>
+  </si>
+  <si>
+    <t>Curso</t>
+  </si>
+  <si>
+    <t>ADS</t>
+  </si>
+  <si>
+    <t>Remotas</t>
+  </si>
+  <si>
+    <t>bbbb</t>
+  </si>
+  <si>
+    <t>xxxxx</t>
+  </si>
+  <si>
+    <t>yyyyy</t>
+  </si>
+  <si>
+    <t>Aula Hibrida (Sim/Nao)</t>
+  </si>
+  <si>
+    <t>Inicio-online</t>
+  </si>
+  <si>
+    <t>Fim-online</t>
+  </si>
+  <si>
+    <t>id-curso-online</t>
+  </si>
+  <si>
+    <t>Escala1</t>
+  </si>
+  <si>
+    <t>ID-Escala-Hibrida</t>
+  </si>
+  <si>
+    <t>id-Escala-hibrida</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,8 +474,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -468,6 +546,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -824,7 +914,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -970,9 +1060,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1033,11 +1121,49 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1059,18 +1185,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1164,8 +1278,8 @@
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>171451</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>781051</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>19051</xdr:rowOff>
     </xdr:to>
@@ -1210,6 +1324,61 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{068FC4EC-9BF2-4457-A0DA-C987EDC0D96D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="1"/>
+          <a:ext cx="781050" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1511,10 +1680,310 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagem 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B247177E-C769-4FDD-B5FB-D6B18B5074C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1"/>
+          <a:ext cx="781050" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagem 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8377DE46-35F7-468D-AE97-C1BF7AAD1A32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1"/>
+          <a:ext cx="781050" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagem 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58E2C505-3A1A-4BFD-A9BF-EF9295015168}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1"/>
+          <a:ext cx="781050" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagem 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB6CE3EE-51FA-4BF8-9F97-82AF76DB96C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1"/>
+          <a:ext cx="781050" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Imagem 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D16C2E0-9D5E-485B-A103-D16CB8160382}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1"/>
+          <a:ext cx="781050" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Imagem 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{573A8569-2BAA-4202-B457-EFA4B1123902}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1"/>
+          <a:ext cx="781050" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1719,7 +2188,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1740,6 +2209,61 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2146E29E-61F4-4468-8F37-8DBF4AC331FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="1"/>
+          <a:ext cx="781050" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>171451</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF9CB4FD-26BA-4C98-B103-C8CBFF8FB228}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2039,8 +2563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A5:D71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2068,6 +2592,9 @@
         <v>10</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="35"/>
+    </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>2</v>
@@ -2075,16 +2602,16 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2095,7 +2622,7 @@
         <v>1234567</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D12" s="4" t="str">
         <f>"Prof"&amp;A12&amp;"-"&amp;B12</f>
@@ -2110,7 +2637,7 @@
         <v>1234568</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D13" s="26" t="str">
         <f t="shared" ref="D13" si="0">"Prof"&amp;A13&amp;"-"&amp;B13</f>
@@ -2474,16 +3001,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F215B73-ACCB-4E5B-B7E9-2E65AA53B0C7}">
-  <dimension ref="A6:D40"/>
+  <dimension ref="A6:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="15.140625" style="1" bestFit="1" customWidth="1"/>
@@ -2493,477 +3020,97 @@
     <col min="112" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="34">
+        <f>parametros!$B$5</f>
         <v>2025</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="34">
+        <f>parametros!$B$6</f>
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="23">
-        <v>2</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="23">
-        <v>4</v>
-      </c>
-      <c r="B13" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
-        <v>5</v>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="59" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="32">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="33">
+        <v>23</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="32">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="33">
+        <v>25</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="23">
-        <v>6</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
-        <v>7</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="23">
-        <v>8</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
-        <v>9</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="23">
-        <v>10</v>
-      </c>
-      <c r="B19" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
-        <v>11</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="23">
-        <v>12</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
-        <v>13</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="23">
-        <v>14</v>
-      </c>
-      <c r="B23" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
-        <v>15</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="23">
-        <v>16</v>
-      </c>
-      <c r="B25" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
-        <v>17</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="23">
-        <v>18</v>
-      </c>
-      <c r="B27" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
-        <v>19</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="23">
-        <v>20</v>
-      </c>
-      <c r="B29" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D29" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
-        <v>21</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="23">
-        <v>22</v>
-      </c>
-      <c r="B31" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="9">
-        <v>23</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="23">
-        <v>24</v>
-      </c>
-      <c r="B33" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D33" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="9">
-        <v>25</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="23">
-        <v>26</v>
-      </c>
-      <c r="B35" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="C35" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="9">
-        <v>27</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="23">
-        <v>28</v>
-      </c>
-      <c r="B37" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="C37" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D37" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="9">
-        <v>29</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="23">
-        <v>30</v>
-      </c>
-      <c r="B39" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="C39" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D39" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="9">
-        <v>31</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>65</v>
-      </c>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="32"/>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="33"/>
+      <c r="B16" s="24"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="32"/>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="33"/>
+      <c r="B18" s="24"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="32"/>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="33"/>
+      <c r="B20" s="24"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:B40" xr:uid="{9FE4B959-7B11-47EC-BE4F-D29AE74B2E8F}">
-      <formula1>"Seg,Ter,Qua,Qui,Sex,Sab,Dom"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:C41" xr:uid="{6EDF8554-1F35-4AE7-921B-DD6F943FDE7E}">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{6EDF8554-1F35-4AE7-921B-DD6F943FDE7E}">
       <formula1>"Sim,Nao"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2973,18 +3120,947 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7E9530-1B40-4B70-870D-BAB8F8FBAD7E}">
-  <dimension ref="A3:WXU24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5AD04F1-4CDB-40D6-8264-1FB73E71E834}">
+  <dimension ref="A5:D79"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="Q24" sqref="B19:Q24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="23.140625" style="1" customWidth="1"/>
+    <col min="13" max="107" width="3.5703125" style="1" customWidth="1"/>
+    <col min="108" max="110" width="26.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="111" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="85" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="85" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="84">
+        <v>45880</v>
+      </c>
+      <c r="D8" s="84">
+        <v>45885</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="85" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="85" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" s="84">
+        <v>45894</v>
+      </c>
+      <c r="D9" s="84">
+        <v>45899</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="85" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" s="85" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="84">
+        <v>45908</v>
+      </c>
+      <c r="D10" s="84">
+        <v>45913</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="85" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" s="85" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="84">
+        <v>45922</v>
+      </c>
+      <c r="D11" s="84">
+        <v>45927</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="85" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" s="85" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="84">
+        <v>45936</v>
+      </c>
+      <c r="D12" s="84">
+        <v>45941</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="85" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="85" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" s="84">
+        <v>45950</v>
+      </c>
+      <c r="D13" s="84">
+        <v>45955</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="85" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" s="85" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="84">
+        <v>45964</v>
+      </c>
+      <c r="D14" s="84">
+        <v>45969</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="85" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" s="85" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" s="84">
+        <v>45978</v>
+      </c>
+      <c r="D15" s="84">
+        <v>45983</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="85" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="85" t="s">
+        <v>117</v>
+      </c>
+      <c r="C16" s="84">
+        <v>46006</v>
+      </c>
+      <c r="D16" s="84">
+        <v>46009</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D17" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D18" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D19" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D20" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D21" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D22" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D23" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D24" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D25" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" s="81"/>
+      <c r="C26" s="83">
+        <v>36526</v>
+      </c>
+      <c r="D26" s="83">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="B27" s="81"/>
+      <c r="C27" s="83">
+        <v>36526</v>
+      </c>
+      <c r="D27" s="83">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" s="81"/>
+      <c r="C28" s="83">
+        <v>36526</v>
+      </c>
+      <c r="D28" s="83">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="B29" s="81"/>
+      <c r="C29" s="83">
+        <v>36526</v>
+      </c>
+      <c r="D29" s="83">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="B30" s="81"/>
+      <c r="C30" s="83">
+        <v>36526</v>
+      </c>
+      <c r="D30" s="83">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" s="81"/>
+      <c r="C31" s="83">
+        <v>36526</v>
+      </c>
+      <c r="D31" s="83">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" s="81"/>
+      <c r="C32" s="83">
+        <v>36526</v>
+      </c>
+      <c r="D32" s="83">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="B33" s="81"/>
+      <c r="C33" s="83">
+        <v>36526</v>
+      </c>
+      <c r="D33" s="83">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="B34" s="81"/>
+      <c r="C34" s="83">
+        <v>36526</v>
+      </c>
+      <c r="D34" s="83">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D35" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D36" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D37" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D38" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D39" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D40" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D41" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D42" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D43" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="B44" s="81"/>
+      <c r="C44" s="83">
+        <v>36526</v>
+      </c>
+      <c r="D44" s="83">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="B45" s="81"/>
+      <c r="C45" s="83">
+        <v>36526</v>
+      </c>
+      <c r="D45" s="83">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46" s="81"/>
+      <c r="C46" s="83">
+        <v>36526</v>
+      </c>
+      <c r="D46" s="83">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="B47" s="81"/>
+      <c r="C47" s="83">
+        <v>36526</v>
+      </c>
+      <c r="D47" s="83">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="B48" s="81"/>
+      <c r="C48" s="83">
+        <v>36526</v>
+      </c>
+      <c r="D48" s="83">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="B49" s="81"/>
+      <c r="C49" s="83">
+        <v>36526</v>
+      </c>
+      <c r="D49" s="83">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="B50" s="81"/>
+      <c r="C50" s="83">
+        <v>36526</v>
+      </c>
+      <c r="D50" s="83">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="B51" s="81"/>
+      <c r="C51" s="83">
+        <v>36526</v>
+      </c>
+      <c r="D51" s="83">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="B52" s="81"/>
+      <c r="C52" s="83">
+        <v>36526</v>
+      </c>
+      <c r="D52" s="83">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D53" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B54" s="2"/>
+      <c r="C54" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D54" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D55" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D56" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B57" s="2"/>
+      <c r="C57" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D57" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B58" s="2"/>
+      <c r="C58" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D58" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B59" s="2"/>
+      <c r="C59" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D59" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B60" s="2"/>
+      <c r="C60" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D60" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B61" s="2"/>
+      <c r="C61" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D61" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="81" t="s">
+        <v>117</v>
+      </c>
+      <c r="B62" s="81"/>
+      <c r="C62" s="83">
+        <v>45880</v>
+      </c>
+      <c r="D62" s="83">
+        <v>45885</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="81" t="s">
+        <v>117</v>
+      </c>
+      <c r="B63" s="81"/>
+      <c r="C63" s="83">
+        <v>45894</v>
+      </c>
+      <c r="D63" s="83">
+        <v>45899</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="81" t="s">
+        <v>117</v>
+      </c>
+      <c r="B64" s="81"/>
+      <c r="C64" s="83">
+        <v>45908</v>
+      </c>
+      <c r="D64" s="83">
+        <v>45913</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="81" t="s">
+        <v>117</v>
+      </c>
+      <c r="B65" s="81"/>
+      <c r="C65" s="83">
+        <v>45922</v>
+      </c>
+      <c r="D65" s="83">
+        <v>45927</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="81" t="s">
+        <v>117</v>
+      </c>
+      <c r="B66" s="81"/>
+      <c r="C66" s="83">
+        <v>45936</v>
+      </c>
+      <c r="D66" s="83">
+        <v>45941</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="81" t="s">
+        <v>117</v>
+      </c>
+      <c r="B67" s="81"/>
+      <c r="C67" s="83">
+        <v>45950</v>
+      </c>
+      <c r="D67" s="83">
+        <v>45955</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="81" t="s">
+        <v>117</v>
+      </c>
+      <c r="B68" s="81"/>
+      <c r="C68" s="83">
+        <v>45964</v>
+      </c>
+      <c r="D68" s="83">
+        <v>45969</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="81" t="s">
+        <v>117</v>
+      </c>
+      <c r="B69" s="81"/>
+      <c r="C69" s="83">
+        <v>45978</v>
+      </c>
+      <c r="D69" s="83">
+        <v>45983</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="81" t="s">
+        <v>117</v>
+      </c>
+      <c r="B70" s="81"/>
+      <c r="C70" s="83">
+        <v>46006</v>
+      </c>
+      <c r="D70" s="83">
+        <v>46009</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B71" s="2"/>
+      <c r="C71" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D71" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B72" s="2"/>
+      <c r="C72" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D72" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B73" s="2"/>
+      <c r="C73" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D73" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B74" s="2"/>
+      <c r="C74" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D74" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B75" s="2"/>
+      <c r="C75" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D75" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B76" s="2"/>
+      <c r="C76" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D76" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B77" s="2"/>
+      <c r="C77" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D77" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B78" s="2"/>
+      <c r="C78" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D78" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B79" s="2"/>
+      <c r="C79" s="82">
+        <v>36526</v>
+      </c>
+      <c r="D79" s="82">
+        <v>36526</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7E9530-1B40-4B70-870D-BAB8F8FBAD7E}">
+  <dimension ref="A3:WXU35"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39" style="1" customWidth="1"/>
     <col min="2" max="2" width="31.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="15.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="11" width="23.140625" style="1" customWidth="1"/>
     <col min="12" max="12" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="26.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -3001,31 +4077,31 @@
     </row>
     <row r="4" spans="1:17 15483:16193" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:17 15483:16193" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:17 15483:16193" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:17 15483:16193" x14ac:dyDescent="0.25">
       <c r="L11" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M11" s="36" t="s">
         <v>26</v>
@@ -3045,7 +4121,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>20</v>
@@ -3100,19 +4176,19 @@
         <v>12</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>8</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
@@ -3884,161 +4960,161 @@
     </row>
     <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="39" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B18" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="G18" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="H18" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="45" t="s">
+      <c r="I18" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="H18" s="44" t="s">
+      <c r="J18" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="K18" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="L18" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="M18" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="L18" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="M18" s="45" t="s">
-        <v>97</v>
-      </c>
-      <c r="N18" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q18" s="45" t="s">
-        <v>101</v>
+      <c r="N18" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="O18" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="P18" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q18" s="38" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="C19" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="D19" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="E19" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="F19" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="G19" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="H19" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="I19" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="J19" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="K19" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="L19" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="M19" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="N19" s="52" t="s">
-        <v>105</v>
-      </c>
-      <c r="O19" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="P19" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q19" s="46" t="s">
-        <v>105</v>
+      <c r="B19" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="G19" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="H19" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="I19" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="J19" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="K19" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="L19" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="M19" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="N19" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="O19" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="P19" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q19" s="37" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="37" t="s">
-        <v>105</v>
-      </c>
-      <c r="C20" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="D20" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="E20" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="F20" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="G20" s="47" t="s">
-        <v>105</v>
-      </c>
-      <c r="H20" s="37" t="s">
-        <v>105</v>
-      </c>
-      <c r="I20" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="J20" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="K20" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="L20" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="M20" s="47" t="s">
-        <v>105</v>
-      </c>
-      <c r="N20" s="53" t="s">
-        <v>105</v>
-      </c>
-      <c r="O20" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="P20" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q20" s="47" t="s">
-        <v>105</v>
+      <c r="B20" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="F20" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="G20" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="H20" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="I20" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="J20" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="K20" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="L20" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="M20" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="N20" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="O20" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="P20" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q20" s="38" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4046,52 +5122,52 @@
         <v>29</v>
       </c>
       <c r="B21" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="C21" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="D21" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="E21" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="F21" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="G21" s="46" t="s">
-        <v>105</v>
+        <v>109</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="F21" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>109</v>
       </c>
       <c r="H21" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="I21" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="J21" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="K21" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="L21" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="M21" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="N21" s="59" t="s">
-        <v>105</v>
-      </c>
-      <c r="O21" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="P21" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q21" s="46" t="s">
-        <v>105</v>
+        <v>109</v>
+      </c>
+      <c r="I21" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="J21" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="K21" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="L21" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="M21" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="N21" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="O21" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="P21" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q21" s="38" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4099,52 +5175,52 @@
         <v>30</v>
       </c>
       <c r="B22" s="37" t="s">
-        <v>105</v>
-      </c>
-      <c r="C22" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="D22" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="E22" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="F22" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="G22" s="47" t="s">
-        <v>105</v>
+        <v>109</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="G22" s="37" t="s">
+        <v>109</v>
       </c>
       <c r="H22" s="37" t="s">
-        <v>105</v>
-      </c>
-      <c r="I22" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="J22" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="K22" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="L22" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="M22" s="47" t="s">
-        <v>105</v>
-      </c>
-      <c r="N22" s="53" t="s">
-        <v>105</v>
-      </c>
-      <c r="O22" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="P22" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q22" s="47" t="s">
-        <v>105</v>
+        <v>109</v>
+      </c>
+      <c r="I22" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="J22" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="K22" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="L22" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="M22" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="N22" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="O22" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="P22" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q22" s="37" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4152,105 +5228,239 @@
         <v>31</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="C23" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="D23" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="E23" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="F23" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="G23" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="H23" s="56" t="s">
-        <v>105</v>
-      </c>
-      <c r="I23" s="57" t="s">
-        <v>105</v>
-      </c>
-      <c r="J23" s="57" t="s">
-        <v>105</v>
-      </c>
-      <c r="K23" s="57" t="s">
-        <v>105</v>
-      </c>
-      <c r="L23" s="57" t="s">
-        <v>105</v>
-      </c>
-      <c r="M23" s="58" t="s">
-        <v>105</v>
-      </c>
-      <c r="N23" s="52" t="s">
-        <v>105</v>
-      </c>
-      <c r="O23" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="P23" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q23" s="46" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="C23" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="E23" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="G23" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="H23" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="I23" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="J23" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="K23" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="L23" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="M23" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="N23" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="O23" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="P23" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q23" s="38" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="48" t="s">
-        <v>105</v>
-      </c>
-      <c r="C24" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="D24" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="E24" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="F24" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="G24" s="50" t="s">
-        <v>105</v>
-      </c>
-      <c r="H24" s="54" t="s">
-        <v>105</v>
-      </c>
-      <c r="I24" s="55" t="s">
-        <v>105</v>
-      </c>
-      <c r="J24" s="55" t="s">
-        <v>105</v>
-      </c>
-      <c r="K24" s="55" t="s">
-        <v>105</v>
-      </c>
-      <c r="L24" s="55" t="s">
-        <v>105</v>
-      </c>
-      <c r="M24" s="55" t="s">
-        <v>105</v>
-      </c>
-      <c r="N24" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="O24" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="P24" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q24" s="50" t="s">
-        <v>105</v>
+      <c r="B24" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="F24" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="G24" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="H24" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="I24" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="J24" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="K24" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="L24" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="M24" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="N24" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="O24" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="P24" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q24" s="37" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="80" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29" s="80" t="s">
+        <v>116</v>
+      </c>
+      <c r="C29" s="80" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" s="80" t="s">
+        <v>113</v>
+      </c>
+      <c r="E29" s="80" t="s">
+        <v>115</v>
+      </c>
+      <c r="F29" s="80" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="str">
+        <f>$G$13</f>
+        <v>Testes de Software</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="81" t="str">
+        <f>$H$13</f>
+        <v>Laboratorio de Engenharia de Software</v>
+      </c>
+      <c r="B31" s="81"/>
+      <c r="C31" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="81" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="str">
+        <f>$I$13</f>
+        <v>Banco de dados I</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="81">
+        <f>$J$13</f>
+        <v>0</v>
+      </c>
+      <c r="B33" s="81"/>
+      <c r="C33" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" s="81" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <f>$K$13</f>
+        <v>0</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="81">
+        <f>$L$13</f>
+        <v>0</v>
+      </c>
+      <c r="B35" s="81"/>
+      <c r="C35" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" s="81" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -4260,14 +5470,29 @@
     <mergeCell ref="H17:M17"/>
     <mergeCell ref="N17:Q17"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B19:Q24">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M13:DD13" xr:uid="{A71FC0CE-E878-409A-AA95-87934C392081}">
+  <conditionalFormatting sqref="N18:Q18">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M13:DD13" xr:uid="{283B38E6-A4BE-487A-B1E3-FD05253F37C1}">
       <formula1>"P,H,."</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F30:F35" xr:uid="{E94E15F7-4B50-4C2C-935D-A16281C16FCB}">
+      <formula1>"Sim,Não"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D30:D35" xr:uid="{EAE438CC-D683-46AE-8064-040D96B923C9}">
+      <formula1>"Seg,Ter,Qua,Qui,Sex,Sab"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E30:E35" xr:uid="{1B6467A8-3632-46EA-BF54-3CC42453005B}">
+      <formula1>"manha,Tarde,Noite"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4275,12 +5500,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6249555E-CACB-4B51-8F35-5416EB9605CE}">
   <dimension ref="A3:WXU24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:Q24"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4304,15 +5529,15 @@
     </row>
     <row r="4" spans="1:17 15483:16193" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:17 15483:16193" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B6" s="2">
         <v>1234568</v>
@@ -4320,15 +5545,15 @@
     </row>
     <row r="7" spans="1:17 15483:16193" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:17 15483:16193" x14ac:dyDescent="0.25">
       <c r="L11" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M11" s="36" t="s">
         <v>26</v>
@@ -4348,7 +5573,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>20</v>
@@ -4403,25 +5628,25 @@
         <v>12</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>8</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>8</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L13" s="8"/>
       <c r="M13" s="2" t="s">
@@ -5191,55 +6416,55 @@
     </row>
     <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="39" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B18" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="G18" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="H18" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="45" t="s">
+      <c r="I18" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="H18" s="44" t="s">
+      <c r="J18" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="K18" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="L18" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="M18" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="N18" s="51" t="s">
         <v>96</v>
       </c>
-      <c r="M18" s="45" t="s">
+      <c r="O18" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="N18" s="51" t="s">
+      <c r="P18" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="O18" s="2" t="s">
+      <c r="Q18" s="45" t="s">
         <v>99</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q18" s="45" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5247,52 +6472,52 @@
         <v>27</v>
       </c>
       <c r="B19" s="38" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C19" s="42" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D19" s="42" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E19" s="42" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F19" s="42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G19" s="46" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H19" s="38" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I19" s="42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J19" s="42" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K19" s="42" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L19" s="42" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M19" s="46" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N19" s="52" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="O19" s="42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="P19" s="42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Q19" s="46" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5300,52 +6525,52 @@
         <v>28</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C20" s="43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D20" s="43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E20" s="43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F20" s="43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G20" s="47" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H20" s="37" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I20" s="43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J20" s="43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K20" s="43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L20" s="43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M20" s="47" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="N20" s="53" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="O20" s="43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="P20" s="43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Q20" s="47" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5353,52 +6578,52 @@
         <v>29</v>
       </c>
       <c r="B21" s="38" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C21" s="42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D21" s="42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E21" s="42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F21" s="42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G21" s="46" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H21" s="38" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I21" s="42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J21" s="42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K21" s="42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L21" s="42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M21" s="46" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="N21" s="52" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="O21" s="42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="P21" s="42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Q21" s="46" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5406,52 +6631,52 @@
         <v>30</v>
       </c>
       <c r="B22" s="37" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C22" s="43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D22" s="43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E22" s="43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F22" s="43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G22" s="47" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H22" s="37" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I22" s="43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J22" s="43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K22" s="43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L22" s="43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M22" s="47" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="N22" s="53" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="O22" s="43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="P22" s="43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Q22" s="47" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5459,52 +6684,52 @@
         <v>31</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C23" s="42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D23" s="42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E23" s="42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F23" s="42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G23" s="46" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H23" s="56" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I23" s="57" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J23" s="57" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K23" s="57" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L23" s="57" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M23" s="58" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="N23" s="52" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="O23" s="42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="P23" s="42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Q23" s="46" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5512,52 +6737,52 @@
         <v>40</v>
       </c>
       <c r="B24" s="48" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C24" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D24" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E24" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F24" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G24" s="50" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H24" s="54" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I24" s="55" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J24" s="55" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K24" s="55" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L24" s="55" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M24" s="55" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="N24" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="O24" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="P24" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Q24" s="50" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -5569,7 +6794,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B19:Q24">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5578,7 +6803,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD0DAE0A-FFDF-4B97-BA23-525E8C8CF0C1}">
   <dimension ref="A6:XFD19"/>
   <sheetViews>
@@ -6470,7 +7695,7 @@
         <v>1234567</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>6</v>
@@ -7499,7 +8724,7 @@
         <v>1234568</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C14" s="26" t="s">
         <v>6</v>
@@ -8528,7 +9753,7 @@
         <v>1234569</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>6</v>
@@ -9557,7 +10782,7 @@
         <v>1234570</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C16" s="26" t="s">
         <v>6</v>
@@ -10586,7 +11811,7 @@
         <v>1234571</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>6</v>
@@ -10905,7 +12130,7 @@
         <v>1234572</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C18" s="26" t="s">
         <v>6</v>
@@ -11224,7 +12449,7 @@
         <v>1234573</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>6</v>
@@ -11545,10 +12770,10 @@
     <mergeCell ref="CH10:DD10"/>
   </mergeCells>
   <conditionalFormatting sqref="N13:DD19">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"H"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11560,4 +12785,503 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C9BA68-DAA8-4EAC-8B39-9BB3CE1F3D04}">
+  <dimension ref="A6:D40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="23.140625" style="1" customWidth="1"/>
+    <col min="14" max="108" width="3.5703125" style="1" customWidth="1"/>
+    <col min="109" max="111" width="26.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="112" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="23">
+        <v>2</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="23">
+        <v>4</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>5</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="23">
+        <v>6</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="23">
+        <v>8</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>9</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="23">
+        <v>10</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>11</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="23">
+        <v>12</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>13</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="23">
+        <v>14</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>15</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="23">
+        <v>16</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>17</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="23">
+        <v>18</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="9">
+        <v>19</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="23">
+        <v>20</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
+        <v>21</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="23">
+        <v>22</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="9">
+        <v>23</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="23">
+        <v>24</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="9">
+        <v>25</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="23">
+        <v>26</v>
+      </c>
+      <c r="B35" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="9">
+        <v>27</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="23">
+        <v>28</v>
+      </c>
+      <c r="B37" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="9">
+        <v>29</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="23">
+        <v>30</v>
+      </c>
+      <c r="B39" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D39" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="9">
+        <v>31</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:C41" xr:uid="{C0E338F9-50F5-4DE7-BC07-CDC52B308538}">
+      <formula1>"Sim,Nao"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:B40" xr:uid="{10C9BBDF-976F-42C0-AB0D-DEADFA7D1B09}">
+      <formula1>"Seg,Ter,Qua,Qui,Sex,Sab,Dom"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>